<commit_message>
changed what is displayed
</commit_message>
<xml_diff>
--- a/data/data_dictionary.xlsx
+++ b/data/data_dictionary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gpain/Documents/Work_Dashboards/Oregon/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{572880DB-5205-3141-9198-6E1C16AF3DBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{422B93CD-0768-9E4F-A737-53856C64E674}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15180" yWindow="920" windowWidth="14900" windowHeight="16940" activeTab="2" xr2:uid="{949A1E6F-A50E-0D47-B806-7BF7EBA35A5B}"/>
+    <workbookView xWindow="15180" yWindow="920" windowWidth="14900" windowHeight="16940" activeTab="1" xr2:uid="{949A1E6F-A50E-0D47-B806-7BF7EBA35A5B}"/>
   </bookViews>
   <sheets>
     <sheet name="ReadMe" sheetId="2" r:id="rId1"/>
@@ -2637,8 +2637,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09851FDF-4334-4E44-81EF-4155DEF57BA3}">
   <dimension ref="A1:K122"/>
   <sheetViews>
-    <sheetView topLeftCell="A60" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B81" sqref="B81"/>
+    <sheetView tabSelected="1" topLeftCell="D20" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4143,10 +4143,10 @@
         <v>28</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G29" s="2" t="s">
         <v>14</v>
@@ -7002,7 +7002,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D1373AD-CAFE-FC46-B12F-4E16ECB9F9F7}">
   <dimension ref="A1:N119"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C104" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="E120" sqref="E120"/>
     </sheetView>
   </sheetViews>

</xml_diff>